<commit_message>
Added more keywords and different distances
</commit_message>
<xml_diff>
--- a/List.xlsx
+++ b/List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\requirements_standards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\requirements_standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61100754-AACF-4FCA-87F2-4CA7CE447F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF713AF-6201-4CB7-A6BD-54AA418444FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="1" xr2:uid="{636553AC-C859-44FA-A214-3636CA836D00}"/>
+    <workbookView xWindow="4290" yWindow="3810" windowWidth="38040" windowHeight="17700" activeTab="1" xr2:uid="{636553AC-C859-44FA-A214-3636CA836D00}"/>
   </bookViews>
   <sheets>
     <sheet name="R_NR" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>Text</t>
   </si>
@@ -103,23 +103,140 @@
     <t>Determining whether to relocate PSA UPF considering the user plane latency requirements provided by the AF (see clause 6.3.6 of TS 23.548 [74]).</t>
   </si>
   <si>
+    <t>LR2_payload</t>
+  </si>
+  <si>
+    <t>LR3_configuration</t>
+  </si>
+  <si>
+    <t>Low end-to-end latency in factory automation, typically means below 10 ms delivery time.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to periodic deterministic communication, shall be less than the end-to-end values listed in TS 22.104, Table 5.2-1: Periodic deterministic communication service performance requirements.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to aperiodic deterministic communication, shall be less than the end-to-end values listed in TS 22.104, Table 5.3-1: Aperiodic deterministic communication service performance requirements.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to mixed traffic communication, shall be less than the end-to-end values listed in TS 22.104, Table 5.5-1: Mixed traffic communication service performance requirements.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget during emergencies, shall be less than the end-to-end values listed in TS 22.104, Table A.4.10-1: Key Performance for uninterrupted MTC service availability.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to primary frequency control, shall be less than the end-to-end values listed in TS 22.104, Table A.4.2-1: Service performance requirements for primary frequency control.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to distributed voltage control, shall be less than the end-to-end values listed in TS 22.104, Table A.4.3-1: Service performance requirements for distributed voltage control.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to smart grid load control, shall be less than the end-to-end values listed in TS 22.104, Table A.4.5-1: Service performance requirements for smart grid millisecond-level precise load control.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to distributed energy storage control, shall be less than the end-to-end values listed in TS 22.104, Table A.4.6-1: Communication service performance requirements ‒ data for distributed energy storage.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to advanced metering, shall be less than the end-to-end values listed in TS 22.104, Table A.4.7-1: Communication KPI for advanced metering.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to smart distribution transformer terminal, shall be less than the end-to-end values listed in TS 22.104, Table A.4.8-1: Key Performance for Smart Distribution Transformer Terminal.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to distributed energy resources and micro-grids, shall be less than the end-to-end values listed in TS 22.104, Table A.4.9-1: Key Performance for Distributed energy resources (DER): using SV (Sampled Values) message.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to wind power plant control, shall be less than the end-to-end values listed in TS 22.104, Table A.5.2-1: Service performance requirements for wind power plant network.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to robotic aided surgery, shall be less than the end-to-end values listed in TS 22.104, Table A.6.2-1: Service performance requirements for motion control and haptic feedback.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to robotic aided diagnosis, shall be less than the end-to-end values listed in TS 22.104, Table A.6.3-1: Service performance requirements for motion control and haptic feedback.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to the support for infrastructure protection of electrical transmission, shall be less than the end-to-end values listed in TS 22.104, chapter 5.6C Support for infrastructure protection of electrical transmission.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to the control of positioning performance requirements, shall be less than the end-to-end values listed in TS 22.104, Table 5.7.1-1: Positioning performance requirements.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to motion control, shall be less than the end-to-end values listed in TS 22.104, Table A.2.2.1-1: Service performance requirements for motion control.</t>
+  </si>
+  <si>
+    <t>Based on operator’s policy, the 5G system shall be able to support a method to predict, monitor network conditions and QoS (e.g. bitrate, latency, reliability) and report to 3rd party along a continuous geographic planned flight path of a UAV at specific times of its expected flight duration. Note: this requirement comes from TS 22.125, tagged as [R-6.2-003]</t>
+  </si>
+  <si>
+    <t>Based on operator’s policy, the 5G system shall be able to provide UTM with the information about geographic areas where UAV service requirements could or could not be met based on predicted network conditions and QoS (e.g. bitrate, latency, reliability). Note: this requirement comes from TS 22.125, tagged as [R-6.8-001]</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to UAV applications, shall be less than the end-to-end values listed in TS 22.125, Table 7.1-1 KPIs for services provided to the UAV applications.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to command and control of UAV operation, shall be less than the end-to-end values listed in TS 22.125, Table 7.2-1 KPIs for command and control of UAV operation.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to UAV positioning performance, shall be less than the end-to-end values listed in TS 22.125, Table 7.3-1: Positioning performance requirements.</t>
+  </si>
+  <si>
+    <t>The 5G system shall support a mechanism to switch between C2 communication modes for UAS operation, e.g. from indirect C2 communication to direct C2 communication, and ensure the disconnect time is below the latency requirements. Note: this requirement comes from TS 22.125, tagged as [R-7.4-001]</t>
+  </si>
+  <si>
+    <t>a) The 3GPP system shall be able to deliver route modification information received from a UTM to a UAS with a latency of less than 500ms. Note: this requirement comes from TS 22.125, tagged as [R-5.2.1-002]
+b) The 3GPP system shall be able to deliver the notifications received from a UTM to a UAV controller with a latency of less than 500ms. Note: this requirement comes from TS 22.125, tagged as [R-5.2.1-003]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 3GPP system shall support a direct UAV to UAV local broadcast communication transport service which can transmit messages with an end-to-end latency of at most 100ms. Note: this requirement comes from TS 22.125, tagged as [R-5.2.2-011] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">High priority communication services, especially their end-to-end latency and availability, shall not be affected by communication services of lower priority running in parallel. Note: this requirement comes from TS 22.289, tagged as [R4.4.2-1] </t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to rail communication scenarios, shall be less than the end-to-end values listed in TS 22.289, Table 5.2.2-1 Performance requirements for rail scenarios – main line.</t>
+  </si>
+  <si>
+    <t>The UPF latency time budget related to rail-bound mass transit communication, shall be less than the end-to-end values listed in TS 22.289, Table 6.2.2.3-1: Characteristic parameters (KPIs) of communication service performance requirements for rail-bound mass transit</t>
+  </si>
+  <si>
+    <t>At least 98% of all packets passing through UPF (UL and DL) shall fulfill the Packet Delay Budget (PDB) values listed in the TS 23.501, table 5.7.4-1: Standardized 5QI to QoS characteristics mapping. Note: PDB defines an upper bound for the time that a packet may be delayed between the UE and the N6 termination point at the UPF.</t>
+  </si>
+  <si>
+    <t>The Slice/Service Type (SST) value for URLLC, stored in PCF, shall be 2.</t>
+  </si>
+  <si>
+    <t>a) MDA capability for E2E latency analytics shall include identifying the type of the E2E latency issue, including, RAN- related latency issue, CN related latency issue, TN-related latency issue, UE-related latency issue and service provider originated latency issue. Note: this requirement comes from TS 28.104, tagged as REQ-LAT_MDA-01.
+b) MDA capability for E2E latency analytics shall include providing the root cause analysis of the E2E latency issue. Note: this requirement comes from TS 28.104, tagged as REQ-LAT_MDA-02
+c) MDA capability for E2E latency analytics shall include providing the recommended actions to solve the E2E latency issue. Note: this requirement comes from TS 28.104, tagged as REQ-LAT_MDA-03</t>
+  </si>
+  <si>
+    <t>NWDAF must be able to utilize Management Data Analytics for E2E latency analysis, as described in TS 28.104, Table 8.4.2.4.2-1: Enabling data for E2E latency analysis.</t>
+  </si>
+  <si>
+    <t>NWDAF must be able to utilize Management Data Analytics for E2E latency analysis, as described in TS 28.104, Table 8.4.2.4.3-1: Analytics output for E2E latency analysis.</t>
+  </si>
+  <si>
+    <t>The downlink latency in gNB-DU shall be calculated as decribed in TS 28.554, chapter 6.3.1.1: Downlink latency in gNB-DU.</t>
+  </si>
+  <si>
+    <t>Energy efficiency of URLLC network slice, based on latency of the network slice, shall be calculated as described in TS 28.554, chapter 6.7.2.3.2 Based on latency of the network slice.</t>
+  </si>
+  <si>
+    <t>Energy efficiency of URLLC network slice, based on both latency and Data Volume (DV) of the network slice, shall be calculated as described in TS 28.554, chapter 6.7.2.3.3 Based on both latency and Data Volume (DV) of the network slice.</t>
+  </si>
+  <si>
+    <t>LR4_calculation</t>
+  </si>
+  <si>
     <t>LR1_signalling</t>
   </si>
   <si>
-    <t>The time contribution of NFx to procedure y, shall be less than z ms, for at least k% of the traffic</t>
-  </si>
-  <si>
-    <t>LR2_payload</t>
-  </si>
-  <si>
-    <t>The UPF contribution to procedure y, shall be less than z ms, for at least k% of the traffic</t>
+    <t>The time budger of AMF for UE triggered service request shall be less than 50ms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,14 +258,31 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <color rgb="FF7030A0"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -186,10 +320,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,10 +671,10 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="111.796875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="111.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -704,13 +844,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D51123B-25DA-4FDA-8A1B-FC0C3B45D7FC}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="35.86328125" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -721,20 +864,308 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="27">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="81">
+      <c r="A3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="81">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="67.5">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="67.5">
+      <c r="A6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="67.5">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="67.5">
+      <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="67.5">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="81">
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="54">
+      <c r="A11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="67.5">
+      <c r="A12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="81">
+      <c r="A13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="67.5">
+      <c r="A14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="67.5">
+      <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="67.5">
+      <c r="A16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="81">
+      <c r="A17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="67.5">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="67.5">
+      <c r="A19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="121.5">
+      <c r="A20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="108">
+      <c r="A21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="67.5">
+      <c r="A22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="67.5">
+      <c r="A23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="67.5">
+      <c r="A24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="94.5">
+      <c r="A25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="135">
+      <c r="A26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="81">
+      <c r="A27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="81">
+      <c r="A28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="67.5">
+      <c r="A29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="94.5">
+      <c r="A30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="108">
+      <c r="A31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="27">
+      <c r="A32" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>25</v>
+      <c r="B32" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="243">
+      <c r="A33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="54">
+      <c r="A34" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="54">
+      <c r="A35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="40.5">
+      <c r="A36" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="67.5">
+      <c r="A37" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="81">
+      <c r="A38" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="27">
+      <c r="A39" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>